<commit_message>
Add model parameter comparison chart
</commit_message>
<xml_diff>
--- a/images/res.xlsx
+++ b/images/res.xlsx
@@ -1,94 +1,430 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAF33C78-0603-47E4-A708-964D852C6F4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:dbsheet="http://web.wps.cn/et/2021/dbsheet">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="11625" xr2:uid="{93A73666-5537-4633-8CD1-54F1413D976B}"/>
+    <workbookView windowWidth="20752" windowHeight="8205" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="PSNR-Set5" sheetId="1" r:id="rId1"/>
+    <sheet name="Params" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="8">
+  <si>
+    <t>SRCNN</t>
+  </si>
+  <si>
+    <t>FSRCNN</t>
+  </si>
+  <si>
+    <t>ESPCN</t>
+  </si>
+  <si>
+    <t>EDSR</t>
+  </si>
+  <si>
+    <t>IMDN</t>
+  </si>
   <si>
     <t>x2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>x3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>x4</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SRCNN</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>FSRCNN</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ESPCN</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>EDSR</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>IMDN</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
+  <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="等线"/>
-      <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="等线"/>
-      <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -96,35 +432,327 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="千位分隔" xfId="1" builtinId="3"/>
+    <cellStyle name="货币" xfId="2" builtinId="4"/>
+    <cellStyle name="百分比" xfId="3" builtinId="5"/>
+    <cellStyle name="千位分隔[0]" xfId="4" builtinId="6"/>
+    <cellStyle name="货币[0]" xfId="5" builtinId="7"/>
+    <cellStyle name="超链接" xfId="6" builtinId="8"/>
+    <cellStyle name="已访问的超链接" xfId="7" builtinId="9"/>
+    <cellStyle name="注释" xfId="8" builtinId="10"/>
+    <cellStyle name="警告文本" xfId="9" builtinId="11"/>
+    <cellStyle name="标题" xfId="10" builtinId="15"/>
+    <cellStyle name="解释性文本" xfId="11" builtinId="53"/>
+    <cellStyle name="标题 1" xfId="12" builtinId="16"/>
+    <cellStyle name="标题 2" xfId="13" builtinId="17"/>
+    <cellStyle name="标题 3" xfId="14" builtinId="18"/>
+    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
+    <cellStyle name="输入" xfId="16" builtinId="20"/>
+    <cellStyle name="输出" xfId="17" builtinId="21"/>
+    <cellStyle name="计算" xfId="18" builtinId="22"/>
+    <cellStyle name="检查单元格" xfId="19" builtinId="23"/>
+    <cellStyle name="链接单元格" xfId="20" builtinId="24"/>
+    <cellStyle name="汇总" xfId="21" builtinId="25"/>
+    <cellStyle name="好" xfId="22" builtinId="26"/>
+    <cellStyle name="差" xfId="23" builtinId="27"/>
+    <cellStyle name="适中" xfId="24" builtinId="28"/>
+    <cellStyle name="强调文字颜色 1" xfId="25" builtinId="29"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="26" builtinId="30"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="27" builtinId="31"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="28" builtinId="32"/>
+    <cellStyle name="强调文字颜色 2" xfId="29" builtinId="33"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="30" builtinId="34"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="31" builtinId="35"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="32" builtinId="36"/>
+    <cellStyle name="强调文字颜色 3" xfId="33" builtinId="37"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="34" builtinId="38"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="35" builtinId="39"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="36" builtinId="40"/>
+    <cellStyle name="强调文字颜色 4" xfId="37" builtinId="41"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="38" builtinId="42"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="39" builtinId="43"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="40" builtinId="44"/>
+    <cellStyle name="强调文字颜色 5" xfId="41" builtinId="45"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="42" builtinId="46"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="43" builtinId="47"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="44" builtinId="48"/>
+    <cellStyle name="强调文字颜色 6" xfId="45" builtinId="49"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="46" builtinId="50"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="zh-CN"/>
   <c:roundedCorners val="0"/>
@@ -144,7 +772,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr lang="zh-CN" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -160,9 +788,11 @@
               <a:rPr lang="en-US" altLang="zh-CN" sz="2000" b="1"/>
               <a:t>Set5-PSNR</a:t>
             </a:r>
+            <a:endParaRPr lang="en-US" altLang="zh-CN" sz="2000" b="1"/>
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -171,26 +801,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="zh-CN"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -203,7 +813,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$2</c:f>
+              <c:f>'PSNR-Set5'!$A$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -224,9 +834,12 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$1:$F$1</c:f>
+              <c:f>'PSNR-Set5'!$B$1:$F$1</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -249,7 +862,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$F$2</c:f>
+              <c:f>'PSNR-Set5'!$B$2:$F$2</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -266,23 +879,18 @@
                   <c:v>36.58</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>36.619999999999997</c:v>
+                  <c:v>36.62</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-F886-48CD-B2DD-151C2C60FFC8}"/>
-            </c:ext>
-          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$3</c:f>
+              <c:f>'PSNR-Set5'!$A$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -303,9 +911,12 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$1:$F$1</c:f>
+              <c:f>'PSNR-Set5'!$B$1:$F$1</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -328,7 +939,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$3:$F$3</c:f>
+              <c:f>'PSNR-Set5'!$B$3:$F$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -350,18 +961,13 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-F886-48CD-B2DD-151C2C60FFC8}"/>
-            </c:ext>
-          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$4</c:f>
+              <c:f>'PSNR-Set5'!$A$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -382,9 +988,12 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$1:$F$1</c:f>
+              <c:f>'PSNR-Set5'!$B$1:$F$1</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -407,7 +1016,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$4:$F$4</c:f>
+              <c:f>'PSNR-Set5'!$B$4:$F$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -429,11 +1038,6 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-F886-48CD-B2DD-151C2C60FFC8}"/>
-            </c:ext>
-          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -475,7 +1079,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr lang="zh-CN" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -487,7 +1091,6 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="840294720"/>
@@ -522,6 +1125,25 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr lang="zh-CN" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
         <c:crossAx val="840294240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
@@ -536,6 +1158,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -549,7 +1172,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr lang="zh-CN" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -561,7 +1184,6 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="zh-CN"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -569,10 +1191,8 @@
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
     <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
+      <c:ext uri="{0b15fc19-7d7d-44ad-8c2d-2c3a37ce22c3}">
+        <chartProps xmlns="https://web.wps.cn/et/2018/main" chartId="{bda3b98f-8115-42d7-a6ba-78f332d5a45c}"/>
       </c:ext>
     </c:extLst>
   </c:chart>
@@ -596,9 +1216,8 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr/>
+        <a:defRPr lang="zh-CN"/>
       </a:pPr>
-      <a:endParaRPr lang="zh-CN"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1154,35 +1773,36 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/customStorage/customStorage.xml><?xml version="1.0" encoding="utf-8"?>
+<customStorage xmlns="https://web.wps.cn/et/2018/main">
+  <book/>
+  <sheets/>
+</customStorage>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>269081</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>382905</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>121443</xdr:rowOff>
+      <xdr:rowOff>130810</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>307181</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>421005</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>45243</xdr:rowOff>
+      <xdr:rowOff>54610</xdr:rowOff>
     </xdr:to>
-    <xdr:graphicFrame macro="">
+    <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="图表 4">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{73601017-74FB-5242-1FF9-0D3BD710868B}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="5" name="图表 4"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
+        <a:off x="1028700" y="1010285"/>
+        <a:ext cx="4558665" cy="2738120"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1238,7 +1858,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -1271,26 +1891,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1323,23 +1926,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1481,105 +2067,195 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05374D03-1E9F-421E-A527-B8629794A325}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:F4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="B1:F1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.85" outlineLevelRow="3" outlineLevelCol="5"/>
+  <sheetData>
+    <row r="1" spans="2:6">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2">
+        <v>34.4</v>
+      </c>
+      <c r="C2">
+        <v>34.35</v>
+      </c>
+      <c r="D2">
+        <v>33.99</v>
+      </c>
+      <c r="E2">
+        <v>36.58</v>
+      </c>
+      <c r="F2">
+        <v>36.62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3">
+        <v>30.48</v>
+      </c>
+      <c r="C3">
+        <v>30.4</v>
+      </c>
+      <c r="D3">
+        <v>30.23</v>
+      </c>
+      <c r="E3">
+        <v>32.17</v>
+      </c>
+      <c r="F3">
+        <v>32.24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4">
+        <v>28.09</v>
+      </c>
+      <c r="C4">
+        <v>28.24</v>
+      </c>
+      <c r="D4">
+        <v>28.04</v>
+      </c>
+      <c r="E4">
+        <v>29.6</v>
+      </c>
+      <c r="F4">
+        <v>29.32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N5" sqref="N5"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="9.02654867256637" defaultRowHeight="13.85" outlineLevelRow="3" outlineLevelCol="5"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="B1" t="s">
+    <row r="1" ht="15.35" spans="1:6">
+      <c r="A1" s="1"/>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D1" t="s">
+    </row>
+    <row r="2" ht="15.35" spans="1:6">
+      <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E1" t="s">
+      <c r="B2" s="1">
+        <v>20099</v>
+      </c>
+      <c r="C2" s="1">
+        <v>24683</v>
+      </c>
+      <c r="D2" s="1">
+        <v>26796</v>
+      </c>
+      <c r="E2" s="1">
+        <v>1332931</v>
+      </c>
+      <c r="F2" s="1">
+        <v>585603</v>
+      </c>
+    </row>
+    <row r="3" ht="15.35" spans="1:6">
+      <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F1" t="s">
+      <c r="B3" s="1">
+        <v>20099</v>
+      </c>
+      <c r="C3" s="1">
+        <v>24683</v>
+      </c>
+      <c r="D3" s="1">
+        <v>31131</v>
+      </c>
+      <c r="E3" s="1">
+        <v>1517571</v>
+      </c>
+      <c r="F3" s="1">
+        <v>698353</v>
+      </c>
+    </row>
+    <row r="4" ht="15.35" spans="1:6">
+      <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2">
-        <v>34.4</v>
-      </c>
-      <c r="C2">
-        <v>34.35</v>
-      </c>
-      <c r="D2">
-        <v>33.99</v>
-      </c>
-      <c r="E2">
-        <v>36.58</v>
-      </c>
-      <c r="F2">
-        <v>36.619999999999997</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3">
-        <v>30.48</v>
-      </c>
-      <c r="C3">
-        <v>30.4</v>
-      </c>
-      <c r="D3">
-        <v>30.23</v>
-      </c>
-      <c r="E3">
-        <v>32.17</v>
-      </c>
-      <c r="F3">
-        <v>32.24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4">
-        <v>28.09</v>
-      </c>
-      <c r="C4">
-        <v>28.24</v>
-      </c>
-      <c r="D4">
-        <v>28.04</v>
-      </c>
-      <c r="E4">
-        <v>29.6</v>
-      </c>
-      <c r="F4">
-        <v>29.32</v>
+      <c r="B4" s="1">
+        <v>20099</v>
+      </c>
+      <c r="C4" s="1">
+        <v>24683</v>
+      </c>
+      <c r="D4" s="1">
+        <v>37200</v>
+      </c>
+      <c r="E4" s="1">
+        <v>1480643</v>
+      </c>
+      <c r="F4" s="1">
+        <v>675803</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>